<commit_message>
automatización de login con usuario válido y agregar productos al carrito
</commit_message>
<xml_diff>
--- a/Plan de pruebas saucedemo.xlsx
+++ b/Plan de pruebas saucedemo.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="standard_user" sheetId="11" r:id="rId1"/>
+    <sheet name="problem_user" sheetId="12" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
   <si>
     <t xml:space="preserve">Observaciones: </t>
   </si>
@@ -413,12 +414,96 @@
   <si>
     <t>Respaldo: Trello: https://trello.com/b/7UMUKc7i/xacademy-qa-automation-cypress</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Precondiciones:
+- Chrome Versión 131.0.6778.86 (Build oficial) (64 bits) 
+Visitar la página: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://www.saucedemo.com/
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Contar con usuario válido: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>problem_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y clave: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secret_sauce</t>
+    </r>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. El botón de cada tarjeta de producto debe cambiar de estilo a rojo y mostrar la leyenda "Remove".                                              2. El botón del carrito de compras debe mostrar un número de productos agregados, en este caso 6.                                          3. Al hacer click en el botón de carrito de compras la app debe dirigirnos al detalle del pedido en la dirección: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.saucedemo.com/cart.html</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -484,14 +569,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,6 +589,18 @@
         <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -617,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -658,9 +749,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -672,8 +760,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,7 +995,10 @@
   <dimension ref="A1:V776"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J4"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -913,18 +1014,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -939,18 +1040,18 @@
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -965,18 +1066,18 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -991,18 +1092,18 @@
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1017,16 +1118,16 @@
       <c r="V4" s="1"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
@@ -1087,13 +1188,13 @@
       <c r="V6" s="1"/>
     </row>
     <row r="7" spans="1:22" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="14" t="s">
@@ -1125,7 +1226,7 @@
       <c r="V7" s="7"/>
     </row>
     <row r="8" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="24" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="15" t="s">
@@ -1138,7 +1239,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>12</v>
@@ -1163,7 +1264,7 @@
       <c r="V8" s="7"/>
     </row>
     <row r="9" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="24" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -1201,7 +1302,7 @@
       <c r="V9" s="7"/>
     </row>
     <row r="10" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="24" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="15" t="s">
@@ -1239,7 +1340,7 @@
       <c r="V10" s="7"/>
     </row>
     <row r="11" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="24" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="15" t="s">
@@ -2063,4 +2164,1179 @@
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="52" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V776"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" customWidth="1"/>
+    <col min="5" max="5" width="55.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="54.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+    </row>
+    <row r="8" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+    </row>
+    <row r="9" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+    </row>
+    <row r="10" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+    </row>
+    <row r="11" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G7:G11">
+      <formula1>"OK,ERROR,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F7:F11">
+      <formula1>"N/A,SI,NO"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
problem-user tests de ingreso, carga de productos y checkout creados
</commit_message>
<xml_diff>
--- a/Plan de pruebas saucedemo.xlsx
+++ b/Plan de pruebas saucedemo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="standard_user" sheetId="11" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
   <si>
     <t xml:space="preserve">Observaciones: </t>
   </si>
@@ -196,20 +196,6 @@
     <t>Realizar checkout</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. El botón de cada tarjeta de producto debe cambiar de estilo a rojo y mostrar la leyenda "Remove".                                              2. El botón del carrito de compras debe mostrar un número de productos agregados, en este caso 6.                                          3. Al hacer click en el boton de carrito de compras la app debe dirigirnos al detalle del pedido en la dirección: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://www.saucedemo.com/cart.html</t>
-    </r>
-  </si>
-  <si>
     <t>4.1.4</t>
   </si>
   <si>
@@ -497,13 +483,161 @@
       </rPr>
       <t>https://www.saucedemo.com/cart.html</t>
     </r>
+  </si>
+  <si>
+    <t>https://trello.com/c/LjvLulxg</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/NS722fd2</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/vL2UteAo</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/7BU0xFQ6</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/CD0OoaMu</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>las imágenes de los productos se repiten</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>En ciertos productos el boton "Add to cart" no funciona.</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/M5yuoEIu</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/G737KNaS</t>
+  </si>
+  <si>
+    <t>4.2.3</t>
+  </si>
+  <si>
+    <t>Pasos:
+1. Escrolear hasta el final de la página observando el detalle de los productos agregados.                                           2. Hacer click en el botón "Checkout".                                 
+3. En la nueva ventana, completar los datos del formulario de checkout con "User" en el imput "First name", "Problem" en el input "Last Name" y 500 en el input "Zip/Postal Code".                                               4. Hacer click en el boton "Continue"</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/akXBXSC5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Precondiciones:
+- Chrome Versión 131.0.6778.86 (Build oficial) (64 bits)                                                        - Haberse logueado con usuario válido 
+- Estar posicionado en la pantalla final del paso 4.2.3. El detalle del pedido de los productos luego del checkout: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://www.saucedemo.com/checkout-step-two.html
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>4.2.4</t>
+  </si>
+  <si>
+    <t>4.2.5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Precondiciones:
+- Chrome Versión 131.0.6778.86 (Build oficial) (64 bits)                                                        - Haberse logueado con usuario válido 
+- Estar posicionado en la pantalla del carrito de compras con los productos seleccionados en el paso 4.2.2: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://www.saucedemo.com/cart.html
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasos:
+1. Escrolear hasta el final de la página observando el detalle de los productos y del pedido.                                           2. Hacer click en el botón "Finish".                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasos:
+1. Hacer click en el botón "Add to cart" una vez en cada producto del catálogo.                                      2. Hacer click en el botón del carrito de compras arriba a la derecha.
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. El botón de cada tarjeta de producto debe cambiar de estilo a rojo y mostrar la leyenda "Remove".                                              2. El botón del carrito de compras debe mostrar el número de productos agregados.                                                               3. Al hacer click en el boton de carrito de compras la app debe dirigirnos al detalle del pedido en la dirección: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.saucedemo.com/cart.html</t>
+    </r>
+  </si>
+  <si>
+    <t>No se puede avanzar hasta solucionar bug en test 4.2.3</t>
+  </si>
+  <si>
+    <t>El formulario de checkout no funciona correctamente. El input "Last name" no responde. Queda pegado al imput "First name" y se activa el warning de "Error: Last Name is required" bloqueando el botón "Continue".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -569,8 +703,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,12 +737,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -637,19 +783,6 @@
       </right>
       <top/>
       <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -708,45 +841,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -760,17 +899,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -788,6 +932,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>998238</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2657476</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1382806</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14790438" y="1314450"/>
+          <a:ext cx="1659238" cy="1354231"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>139374</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2741139</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1552574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14801850" y="2825424"/>
+          <a:ext cx="1731489" cy="1413200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>40481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2990850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1552574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14363700" y="4317206"/>
+          <a:ext cx="2419350" cy="1512093"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -994,11 +1275,11 @@
   </sheetPr>
   <dimension ref="A1:V776"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1014,18 +1295,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
+      <c r="A1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1040,18 +1321,18 @@
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="A2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1066,18 +1347,18 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
+      <c r="A3" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1092,18 +1373,18 @@
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="19"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1117,17 +1398,17 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19" t="s">
+    <row r="5" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
@@ -1143,35 +1424,35 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
     </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K6" s="1"/>
@@ -1188,194 +1469,204 @@
       <c r="V6" s="1"/>
     </row>
     <row r="7" spans="1:22" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
     </row>
     <row r="8" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
     </row>
     <row r="9" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="C9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
     </row>
     <row r="10" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="A10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
     </row>
     <row r="11" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2170,11 +2461,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V776"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2190,18 +2481,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
+      <c r="A1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -2216,18 +2507,18 @@
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="A2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -2242,18 +2533,18 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
+      <c r="A3" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2268,18 +2559,18 @@
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="19"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2294,16 +2585,16 @@
       <c r="V4" s="1"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
@@ -2319,35 +2610,35 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
     </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K6" s="1"/>
@@ -2365,193 +2656,209 @@
     </row>
     <row r="7" spans="1:22" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="C7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
+      <c r="E7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
     </row>
     <row r="8" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
+      <c r="D8" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
     </row>
     <row r="9" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="C9" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
     </row>
     <row r="10" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="F10" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
+      <c r="G10" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
     </row>
     <row r="11" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="F11" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
+      <c r="G11" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3338,5 +3645,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tests problem_user agregar productos y realizar checkout realizados y bugs reportados
</commit_message>
<xml_diff>
--- a/Plan de pruebas saucedemo.xlsx
+++ b/Plan de pruebas saucedemo.xlsx
@@ -613,8 +613,14 @@
 </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. El botón de cada tarjeta de producto debe cambiar de estilo a rojo y mostrar la leyenda "Remove".                                              2. El botón del carrito de compras debe mostrar el número de productos agregados.                                                               3. Al hacer click en el boton de carrito de compras la app debe dirigirnos al detalle del pedido en la dirección: </t>
+    <t>No se puede avanzar hasta solucionar bug en test 4.2.3</t>
+  </si>
+  <si>
+    <t>El formulario de checkout no funciona correctamente. El input "Last name" no responde. Queda pegado al imput "First name" y se activa el warning de "Error: Last Name is required" bloqueando el botón "Continue".</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. El botón de cada tarjeta de producto debe cambiar de estilo a rojo y mostrar la leyenda "Remove".                                              2. El botón del carrito de compras debe mostrar el número de productos agregados.                                                               3. Al hacer click en el botón de carrito de compras la app debe dirigirnos al detalle del pedido en la dirección: </t>
     </r>
     <r>
       <rPr>
@@ -625,12 +631,6 @@
       </rPr>
       <t>https://www.saucedemo.com/cart.html</t>
     </r>
-  </si>
-  <si>
-    <t>No se puede avanzar hasta solucionar bug en test 4.2.3</t>
-  </si>
-  <si>
-    <t>El formulario de checkout no funciona correctamente. El input "Last name" no responde. Queda pegado al imput "First name" y se activa el warning de "Error: Last Name is required" bloqueando el botón "Continue".</t>
   </si>
 </sst>
 </file>
@@ -888,17 +888,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -916,6 +905,17 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1295,18 +1295,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1321,18 +1321,18 @@
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1347,18 +1347,18 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1373,18 +1373,18 @@
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1399,16 +1399,16 @@
       <c r="V4" s="1"/>
     </row>
     <row r="5" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
@@ -2462,10 +2462,10 @@
   <dimension ref="A1:V776"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2481,18 +2481,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -2507,18 +2507,18 @@
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -2533,18 +2533,18 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2559,18 +2559,18 @@
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2585,16 +2585,16 @@
       <c r="V4" s="1"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
@@ -2655,7 +2655,7 @@
       <c r="V6" s="1"/>
     </row>
     <row r="7" spans="1:22" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="18" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -2697,7 +2697,7 @@
       <c r="V7" s="6"/>
     </row>
     <row r="8" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="17" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -2710,7 +2710,7 @@
         <v>64</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>12</v>
@@ -2739,13 +2739,13 @@
       <c r="V8" s="6"/>
     </row>
     <row r="9" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="17" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="19" t="s">
         <v>62</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -2762,7 +2762,7 @@
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>58</v>
@@ -2781,13 +2781,13 @@
       <c r="V9" s="6"/>
     </row>
     <row r="10" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="19" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -2796,15 +2796,15 @@
       <c r="E10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="20" t="s">
         <v>41</v>
       </c>
       <c r="H10" s="9"/>
-      <c r="I10" s="26" t="s">
-        <v>66</v>
+      <c r="I10" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
@@ -2821,10 +2821,10 @@
       <c r="V10" s="6"/>
     </row>
     <row r="11" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="22" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -2836,15 +2836,15 @@
       <c r="E11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="20" t="s">
         <v>41</v>
       </c>
       <c r="H11" s="9"/>
-      <c r="I11" s="26" t="s">
-        <v>66</v>
+      <c r="I11" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>

</xml_diff>